<commit_message>
cleaed data from version2 of numDistractor/basiclevel experiment and added basiclevel graphs
</commit_message>
<xml_diff>
--- a/Caroline/Stimuli_Experiment2_version2/stimuliOverview.xlsx
+++ b/Caroline/Stimuli_Experiment2_version2/stimuliOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4220" yWindow="0" windowWidth="13680" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="-1060" yWindow="20" windowWidth="13680" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="272">
   <si>
     <t>target</t>
   </si>
@@ -762,9 +762,6 @@
     <t>bison</t>
   </si>
   <si>
-    <t>chick</t>
-  </si>
-  <si>
     <t>elephant</t>
   </si>
   <si>
@@ -826,6 +823,18 @@
   </si>
   <si>
     <t>rabbit</t>
+  </si>
+  <si>
+    <t>hamster</t>
+  </si>
+  <si>
+    <t>Frequencies_version2:</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>catfish</t>
   </si>
 </sst>
 </file>
@@ -900,8 +909,100 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -993,7 +1094,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1034,6 +1135,52 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1074,6 +1221,52 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1403,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ58"/>
+  <dimension ref="A1:BC58"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AN33" sqref="AN33"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="AS18" workbookViewId="0">
+      <selection activeCell="AY26" sqref="AY26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1414,9 +1607,11 @@
     <col min="24" max="24" width="13.6640625" customWidth="1"/>
     <col min="25" max="25" width="17.5" customWidth="1"/>
     <col min="27" max="27" width="28.6640625" customWidth="1"/>
+    <col min="51" max="51" width="14.33203125" customWidth="1"/>
+    <col min="53" max="53" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:55">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1471,6 +1666,9 @@
       <c r="Y1" t="s">
         <v>206</v>
       </c>
+      <c r="Z1" t="s">
+        <v>270</v>
+      </c>
       <c r="AA1" t="s">
         <v>203</v>
       </c>
@@ -1493,10 +1691,25 @@
         <v>215</v>
       </c>
       <c r="AN1" t="s">
-        <v>256</v>
+        <v>255</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>269</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>204</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>270</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:55">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1581,10 +1794,28 @@
         <v>101</v>
       </c>
       <c r="AQ2" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AX2">
+        <v>39951249</v>
+      </c>
+      <c r="AY2">
+        <v>1.1765540538854234E-4</v>
+      </c>
+      <c r="AZ2">
+        <v>1960</v>
+      </c>
+      <c r="BA2">
+        <v>2341981521</v>
+      </c>
+      <c r="BC2">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:55">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1666,10 +1897,22 @@
         <v>11</v>
       </c>
       <c r="AQ3" t="s">
-        <v>261</v>
+        <v>260</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AZ3">
+        <v>1961</v>
+      </c>
+      <c r="BA3">
+        <v>2567977722</v>
+      </c>
+      <c r="BC3">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:55">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1751,10 +1994,22 @@
         <v>12</v>
       </c>
       <c r="AQ4" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>243</v>
+      </c>
+      <c r="AZ4">
+        <v>1962</v>
+      </c>
+      <c r="BA4">
+        <v>2818694749</v>
+      </c>
+      <c r="BC4">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:55">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1836,10 +2091,22 @@
         <v>13</v>
       </c>
       <c r="AQ5" t="s">
-        <v>263</v>
+        <v>262</v>
+      </c>
+      <c r="AW5" t="s">
+        <v>214</v>
+      </c>
+      <c r="AZ5">
+        <v>1963</v>
+      </c>
+      <c r="BA5">
+        <v>2955051696</v>
+      </c>
+      <c r="BC5">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:55">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1905,8 +2172,20 @@
       <c r="AM6" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="AW6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AZ6">
+        <v>1964</v>
+      </c>
+      <c r="BA6">
+        <v>2931038992</v>
+      </c>
+      <c r="BC6">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:55">
       <c r="W7" t="s">
         <v>147</v>
       </c>
@@ -1938,8 +2217,20 @@
       <c r="AM7" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="AW7" t="s">
+        <v>212</v>
+      </c>
+      <c r="AZ7">
+        <v>1965</v>
+      </c>
+      <c r="BA7">
+        <v>3300623502</v>
+      </c>
+      <c r="BC7">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:55">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2009,7 +2300,7 @@
         <v>339561526035</v>
       </c>
       <c r="AH8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="AI8" t="s">
         <v>38</v>
@@ -2020,8 +2311,20 @@
       <c r="AM8" s="3" t="s">
         <v>173</v>
       </c>
+      <c r="AW8" t="s">
+        <v>38</v>
+      </c>
+      <c r="AZ8">
+        <v>1966</v>
+      </c>
+      <c r="BA8">
+        <v>3466842517</v>
+      </c>
+      <c r="BC8">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:55">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2091,7 +2394,7 @@
         <v>339561526035</v>
       </c>
       <c r="AH9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="AI9" t="s">
         <v>38</v>
@@ -2102,8 +2405,20 @@
       <c r="AM9" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="AW9" t="s">
+        <v>271</v>
+      </c>
+      <c r="AZ9">
+        <v>1967</v>
+      </c>
+      <c r="BA9">
+        <v>3658119990</v>
+      </c>
+      <c r="BC9">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:55">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2185,10 +2500,28 @@
         <v>228</v>
       </c>
       <c r="AM10" t="s">
-        <v>253</v>
+        <v>252</v>
+      </c>
+      <c r="AW10" t="s">
+        <v>150</v>
+      </c>
+      <c r="AX10">
+        <v>7987510</v>
+      </c>
+      <c r="AY10">
+        <v>2.3523012436858629E-5</v>
+      </c>
+      <c r="AZ10">
+        <v>1968</v>
+      </c>
+      <c r="BA10">
+        <v>3968752101</v>
+      </c>
+      <c r="BC10">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:55">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2267,10 +2600,22 @@
         <v>244</v>
       </c>
       <c r="AM11" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>237</v>
+      </c>
+      <c r="AZ11">
+        <v>1969</v>
+      </c>
+      <c r="BA11">
+        <v>3942222509</v>
+      </c>
+      <c r="BC11">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:55">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2328,10 +2673,22 @@
         <v>244</v>
       </c>
       <c r="AM12" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="AW12" t="s">
+        <v>241</v>
+      </c>
+      <c r="AZ12">
+        <v>1970</v>
+      </c>
+      <c r="BA12">
+        <v>4086393350</v>
+      </c>
+      <c r="BC12">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:55">
       <c r="W13" t="s">
         <v>48</v>
       </c>
@@ -2363,8 +2720,20 @@
       <c r="AM13" s="3" t="s">
         <v>74</v>
       </c>
+      <c r="AW13" t="s">
+        <v>221</v>
+      </c>
+      <c r="AZ13">
+        <v>1971</v>
+      </c>
+      <c r="BA13">
+        <v>4058576649</v>
+      </c>
+      <c r="BC13">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:55">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2443,13 +2812,32 @@
         <v>150</v>
       </c>
       <c r="AL14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="AM14" s="3" t="s">
         <v>144</v>
       </c>
+      <c r="AW14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="AX14">
+        <v>1142904</v>
+      </c>
+      <c r="AY14">
+        <f>AX14/BC13</f>
+        <v>3.3658230169521507E-6</v>
+      </c>
+      <c r="AZ14">
+        <v>1972</v>
+      </c>
+      <c r="BA14">
+        <v>4174172415</v>
+      </c>
+      <c r="BC14">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="15" spans="1:43">
+    <row r="15" spans="1:55">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2530,8 +2918,26 @@
       <c r="AM15" s="3" t="s">
         <v>145</v>
       </c>
+      <c r="AW15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AX15">
+        <v>49602</v>
+      </c>
+      <c r="AY15">
+        <v>1.4607661998458365E-7</v>
+      </c>
+      <c r="AZ15">
+        <v>1973</v>
+      </c>
+      <c r="BA15">
+        <v>4058707895</v>
+      </c>
+      <c r="BC15">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="16" spans="1:43">
+    <row r="16" spans="1:55">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2612,8 +3018,20 @@
       <c r="AM16" s="3" t="s">
         <v>153</v>
       </c>
+      <c r="AW16" t="s">
+        <v>242</v>
+      </c>
+      <c r="AZ16">
+        <v>1974</v>
+      </c>
+      <c r="BA16">
+        <v>4045487401</v>
+      </c>
+      <c r="BC16">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="17" spans="1:39">
+    <row r="17" spans="1:55">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2694,8 +3112,27 @@
       <c r="AM17" s="3" t="s">
         <v>89</v>
       </c>
+      <c r="AW17" t="s">
+        <v>193</v>
+      </c>
+      <c r="AX17">
+        <v>21789518</v>
+      </c>
+      <c r="AY17">
+        <f>AX17/BC16</f>
+        <v>6.4169572608629595E-5</v>
+      </c>
+      <c r="AZ17">
+        <v>1975</v>
+      </c>
+      <c r="BA17">
+        <v>4104379941</v>
+      </c>
+      <c r="BC17">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="18" spans="1:39">
+    <row r="18" spans="1:55">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2758,8 +3195,20 @@
       <c r="AM18" t="s">
         <v>98</v>
       </c>
+      <c r="AW18" t="s">
+        <v>144</v>
+      </c>
+      <c r="AZ18">
+        <v>1976</v>
+      </c>
+      <c r="BA18">
+        <v>4242326406</v>
+      </c>
+      <c r="BC18">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="19" spans="1:39">
+    <row r="19" spans="1:55">
       <c r="W19" t="s">
         <v>7</v>
       </c>
@@ -2791,8 +3240,20 @@
       <c r="AM19" t="s">
         <v>99</v>
       </c>
+      <c r="AW19" t="s">
+        <v>231</v>
+      </c>
+      <c r="AZ19">
+        <v>1977</v>
+      </c>
+      <c r="BA19">
+        <v>4314577619</v>
+      </c>
+      <c r="BC19">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="20" spans="1:39">
+    <row r="20" spans="1:55">
       <c r="A20">
         <v>4</v>
       </c>
@@ -2873,8 +3334,20 @@
       <c r="AM20" t="s">
         <v>100</v>
       </c>
+      <c r="AW20" t="s">
+        <v>213</v>
+      </c>
+      <c r="AZ20">
+        <v>1978</v>
+      </c>
+      <c r="BA20">
+        <v>4365839878</v>
+      </c>
+      <c r="BC20">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="21" spans="1:39">
+    <row r="21" spans="1:55">
       <c r="A21">
         <v>4</v>
       </c>
@@ -2953,10 +3426,29 @@
         <v>9</v>
       </c>
       <c r="AM21" t="s">
-        <v>268</v>
+        <v>267</v>
+      </c>
+      <c r="AW21" t="s">
+        <v>199</v>
+      </c>
+      <c r="AX21">
+        <v>16497919</v>
+      </c>
+      <c r="AY21">
+        <f>AX21/BC20</f>
+        <v>4.8585949040350033E-5</v>
+      </c>
+      <c r="AZ21">
+        <v>1979</v>
+      </c>
+      <c r="BA21">
+        <v>4528331460</v>
+      </c>
+      <c r="BC21">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="22" spans="1:39">
+    <row r="22" spans="1:55">
       <c r="A22">
         <v>4</v>
       </c>
@@ -3040,8 +3532,26 @@
       <c r="AM22" s="3" t="s">
         <v>92</v>
       </c>
+      <c r="AW22" t="s">
+        <v>19</v>
+      </c>
+      <c r="AX22">
+        <v>6098822</v>
+      </c>
+      <c r="AY22">
+        <v>1.7960874635047345E-5</v>
+      </c>
+      <c r="AZ22">
+        <v>1980</v>
+      </c>
+      <c r="BA22">
+        <v>4611609946</v>
+      </c>
+      <c r="BC22">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="23" spans="1:39">
+    <row r="23" spans="1:55">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3123,8 +3633,27 @@
       <c r="AM23" s="3" t="s">
         <v>132</v>
       </c>
+      <c r="AW23" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AX23">
+        <v>97790</v>
+      </c>
+      <c r="AY23">
+        <f>AX23/BC22</f>
+        <v>2.8798904617338887E-7</v>
+      </c>
+      <c r="AZ23">
+        <v>1981</v>
+      </c>
+      <c r="BA23">
+        <v>4627406112</v>
+      </c>
+      <c r="BC23">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="24" spans="1:39">
+    <row r="24" spans="1:55">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3185,8 +3714,20 @@
       <c r="AM24" s="3" t="s">
         <v>133</v>
       </c>
+      <c r="AW24" t="s">
+        <v>239</v>
+      </c>
+      <c r="AZ24">
+        <v>1982</v>
+      </c>
+      <c r="BA24">
+        <v>4839530894</v>
+      </c>
+      <c r="BC24">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="25" spans="1:39">
+    <row r="25" spans="1:55">
       <c r="W25" t="s">
         <v>194</v>
       </c>
@@ -3219,8 +3760,20 @@
       <c r="AM25" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="AW25" t="s">
+        <v>216</v>
+      </c>
+      <c r="AZ25">
+        <v>1983</v>
+      </c>
+      <c r="BA25">
+        <v>4982167985</v>
+      </c>
+      <c r="BC25">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="26" spans="1:39">
+    <row r="26" spans="1:55">
       <c r="A26">
         <v>5</v>
       </c>
@@ -3304,8 +3857,20 @@
       <c r="AM26" t="s">
         <v>246</v>
       </c>
+      <c r="AW26" t="s">
+        <v>223</v>
+      </c>
+      <c r="AZ26">
+        <v>1984</v>
+      </c>
+      <c r="BA26">
+        <v>5309222580</v>
+      </c>
+      <c r="BC26">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="27" spans="1:39">
+    <row r="27" spans="1:55">
       <c r="A27">
         <v>5</v>
       </c>
@@ -3384,10 +3949,22 @@
         <v>9</v>
       </c>
       <c r="AM27" t="s">
-        <v>247</v>
+        <v>268</v>
+      </c>
+      <c r="AW27" t="s">
+        <v>235</v>
+      </c>
+      <c r="AZ27">
+        <v>1985</v>
+      </c>
+      <c r="BA27">
+        <v>5475269397</v>
+      </c>
+      <c r="BC27">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="28" spans="1:39">
+    <row r="28" spans="1:55">
       <c r="A28">
         <v>5</v>
       </c>
@@ -3466,10 +4043,22 @@
         <v>9</v>
       </c>
       <c r="AM28" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="AW28" t="s">
+        <v>232</v>
+      </c>
+      <c r="AZ28">
+        <v>1986</v>
+      </c>
+      <c r="BA28">
+        <v>5793946882</v>
+      </c>
+      <c r="BC28">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="29" spans="1:39">
+    <row r="29" spans="1:55">
       <c r="A29">
         <v>5</v>
       </c>
@@ -3548,10 +4137,29 @@
         <v>9</v>
       </c>
       <c r="AM29" t="s">
-        <v>249</v>
+        <v>248</v>
+      </c>
+      <c r="AW29" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="AX29">
+        <v>76741</v>
+      </c>
+      <c r="AY29">
+        <f>AX29/BC28</f>
+        <v>2.2600028011444968E-7</v>
+      </c>
+      <c r="AZ29">
+        <v>1987</v>
+      </c>
+      <c r="BA29">
+        <v>5936558026</v>
+      </c>
+      <c r="BC29">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="30" spans="1:39">
+    <row r="30" spans="1:55">
       <c r="A30">
         <v>5</v>
       </c>
@@ -3609,13 +4217,25 @@
         <v>9</v>
       </c>
       <c r="AL30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="AM30" t="s">
-        <v>250</v>
+        <v>249</v>
+      </c>
+      <c r="AW30" t="s">
+        <v>225</v>
+      </c>
+      <c r="AZ30">
+        <v>1988</v>
+      </c>
+      <c r="BA30">
+        <v>6191886939</v>
+      </c>
+      <c r="BC30">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="31" spans="1:39">
+    <row r="31" spans="1:55">
       <c r="W31" t="s">
         <v>67</v>
       </c>
@@ -3645,10 +4265,22 @@
         <v>9</v>
       </c>
       <c r="AM31" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="AW31" t="s">
+        <v>226</v>
+      </c>
+      <c r="AZ31">
+        <v>1989</v>
+      </c>
+      <c r="BA31">
+        <v>6549339038</v>
+      </c>
+      <c r="BC31">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="32" spans="1:39">
+    <row r="32" spans="1:55">
       <c r="A32">
         <v>6</v>
       </c>
@@ -3727,10 +4359,22 @@
         <v>9</v>
       </c>
       <c r="AM32" t="s">
-        <v>252</v>
+        <v>251</v>
+      </c>
+      <c r="AW32" t="s">
+        <v>256</v>
+      </c>
+      <c r="AZ32">
+        <v>1990</v>
+      </c>
+      <c r="BA32">
+        <v>7075013106</v>
+      </c>
+      <c r="BC32">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="33" spans="1:39">
+    <row r="33" spans="1:55">
       <c r="A33">
         <v>6</v>
       </c>
@@ -3803,7 +4447,7 @@
         <v>339561526035</v>
       </c>
       <c r="AH33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AI33" t="s">
         <v>213</v>
@@ -3812,10 +4456,22 @@
         <v>9</v>
       </c>
       <c r="AM33" t="s">
-        <v>267</v>
+        <v>266</v>
+      </c>
+      <c r="AW33" t="s">
+        <v>220</v>
+      </c>
+      <c r="AZ33">
+        <v>1991</v>
+      </c>
+      <c r="BA33">
+        <v>6895715366</v>
+      </c>
+      <c r="BC33">
+        <v>339561526035</v>
       </c>
     </row>
-    <row r="34" spans="1:39">
+    <row r="34" spans="1:55">
       <c r="A34">
         <v>6</v>
       </c>
@@ -3899,13 +4555,25 @@
         <v>19</v>
       </c>
       <c r="AL34" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="AM34" s="3" t="s">
         <v>34</v>
       </c>
+      <c r="AW34" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ34">
+        <v>1992</v>
+      </c>
+      <c r="BA34">
+        <v>7596808027</v>
+      </c>
+      <c r="BC34">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="35" spans="1:39">
+    <row r="35" spans="1:55">
       <c r="A35">
         <v>6</v>
       </c>
@@ -3986,8 +4654,20 @@
       <c r="AM35" s="3" t="s">
         <v>167</v>
       </c>
+      <c r="AW35" t="s">
+        <v>240</v>
+      </c>
+      <c r="AZ35">
+        <v>1993</v>
+      </c>
+      <c r="BA35">
+        <v>7492130348</v>
+      </c>
+      <c r="BC35">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="36" spans="1:39">
+    <row r="36" spans="1:55">
       <c r="A36">
         <v>6</v>
       </c>
@@ -4050,8 +4730,20 @@
       <c r="AM36" s="3" t="s">
         <v>166</v>
       </c>
+      <c r="AW36" t="s">
+        <v>234</v>
+      </c>
+      <c r="AZ36">
+        <v>1994</v>
+      </c>
+      <c r="BA36">
+        <v>8027353540</v>
+      </c>
+      <c r="BC36">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="37" spans="1:39">
+    <row r="37" spans="1:55">
       <c r="B37" t="s">
         <v>182</v>
       </c>
@@ -4089,8 +4781,26 @@
       <c r="AM37" s="3" t="s">
         <v>169</v>
       </c>
+      <c r="AW37" t="s">
+        <v>201</v>
+      </c>
+      <c r="AX37">
+        <v>52852109</v>
+      </c>
+      <c r="AY37">
+        <v>1.5564810777341222E-4</v>
+      </c>
+      <c r="AZ37">
+        <v>1995</v>
+      </c>
+      <c r="BA37">
+        <v>8276258599</v>
+      </c>
+      <c r="BC37">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="38" spans="1:39">
+    <row r="38" spans="1:55">
       <c r="A38">
         <v>7</v>
       </c>
@@ -4156,8 +4866,20 @@
       <c r="AC38">
         <v>339561526035</v>
       </c>
+      <c r="AW38" t="s">
+        <v>217</v>
+      </c>
+      <c r="AZ38">
+        <v>1996</v>
+      </c>
+      <c r="BA38">
+        <v>8745049453</v>
+      </c>
+      <c r="BC38">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="39" spans="1:39">
+    <row r="39" spans="1:55">
       <c r="A39">
         <v>7</v>
       </c>
@@ -4223,8 +4945,20 @@
       <c r="AC39">
         <v>339561526035</v>
       </c>
+      <c r="AW39" t="s">
+        <v>229</v>
+      </c>
+      <c r="AZ39">
+        <v>1997</v>
+      </c>
+      <c r="BA39">
+        <v>8979708108</v>
+      </c>
+      <c r="BC39">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="40" spans="1:39">
+    <row r="40" spans="1:55">
       <c r="A40">
         <v>7</v>
       </c>
@@ -4287,8 +5021,27 @@
       <c r="AC40">
         <v>339561526035</v>
       </c>
+      <c r="AW40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX40">
+        <v>121280</v>
+      </c>
+      <c r="AY40">
+        <f t="shared" ref="AY40" si="1">AX40/BC40</f>
+        <v>3.5716649473267821E-7</v>
+      </c>
+      <c r="AZ40">
+        <v>1998</v>
+      </c>
+      <c r="BA40">
+        <v>9406708249</v>
+      </c>
+      <c r="BC40">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="41" spans="1:39">
+    <row r="41" spans="1:55">
       <c r="A41">
         <v>7</v>
       </c>
@@ -4351,8 +5104,27 @@
       <c r="AC41">
         <v>339561526035</v>
       </c>
+      <c r="AW41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="AX41">
+        <v>8595412</v>
+      </c>
+      <c r="AY41">
+        <f t="shared" ref="AY41" si="2">AX41/BC41</f>
+        <v>2.5313268262064634E-5</v>
+      </c>
+      <c r="AZ41">
+        <v>1999</v>
+      </c>
+      <c r="BA41">
+        <v>9997156197</v>
+      </c>
+      <c r="BC41">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="42" spans="1:39">
+    <row r="42" spans="1:55">
       <c r="A42">
         <v>7</v>
       </c>
@@ -4400,8 +5172,20 @@
       <c r="AC42">
         <v>339561526035</v>
       </c>
+      <c r="AW42" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ42">
+        <v>2000</v>
+      </c>
+      <c r="BA42">
+        <v>11190986329</v>
+      </c>
+      <c r="BC42">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="43" spans="1:39">
+    <row r="43" spans="1:55">
       <c r="W43" t="s">
         <v>37</v>
       </c>
@@ -4421,8 +5205,20 @@
       <c r="AC43">
         <v>339561526035</v>
       </c>
+      <c r="AW43" t="s">
+        <v>224</v>
+      </c>
+      <c r="AZ43">
+        <v>2001</v>
+      </c>
+      <c r="BA43">
+        <v>11349375656</v>
+      </c>
+      <c r="BC43">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="44" spans="1:39">
+    <row r="44" spans="1:55">
       <c r="A44">
         <v>8</v>
       </c>
@@ -4491,8 +5287,20 @@
       <c r="AC44">
         <v>339561526035</v>
       </c>
+      <c r="AW44" t="s">
+        <v>244</v>
+      </c>
+      <c r="AZ44">
+        <v>2002</v>
+      </c>
+      <c r="BA44">
+        <v>12519922882</v>
+      </c>
+      <c r="BC44">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="45" spans="1:39">
+    <row r="45" spans="1:55">
       <c r="A45">
         <v>8</v>
       </c>
@@ -4561,8 +5369,20 @@
       <c r="AC45">
         <v>339561526035</v>
       </c>
+      <c r="AW45" t="s">
+        <v>257</v>
+      </c>
+      <c r="AZ45">
+        <v>2003</v>
+      </c>
+      <c r="BA45">
+        <v>13632028136</v>
+      </c>
+      <c r="BC45">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="46" spans="1:39">
+    <row r="46" spans="1:55">
       <c r="A46">
         <v>8</v>
       </c>
@@ -4631,8 +5451,27 @@
       <c r="AC46">
         <v>339561526035</v>
       </c>
+      <c r="AW46" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AX46">
+        <v>583171</v>
+      </c>
+      <c r="AY46">
+        <f t="shared" ref="AY46" si="3">AX46/BC46</f>
+        <v>1.7174236634214271E-6</v>
+      </c>
+      <c r="AZ46">
+        <v>2004</v>
+      </c>
+      <c r="BA46">
+        <v>14705541576</v>
+      </c>
+      <c r="BC46">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="47" spans="1:39">
+    <row r="47" spans="1:55">
       <c r="A47">
         <v>8</v>
       </c>
@@ -4701,8 +5540,20 @@
       <c r="AC47">
         <v>339561526035</v>
       </c>
+      <c r="AW47" t="s">
+        <v>222</v>
+      </c>
+      <c r="AZ47">
+        <v>2005</v>
+      </c>
+      <c r="BA47">
+        <v>14425183957</v>
+      </c>
+      <c r="BC47">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="48" spans="1:39">
+    <row r="48" spans="1:55">
       <c r="A48">
         <v>8</v>
       </c>
@@ -4750,8 +5601,20 @@
       <c r="AC48">
         <v>339561526035</v>
       </c>
+      <c r="AW48" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ48">
+        <v>2006</v>
+      </c>
+      <c r="BA48">
+        <v>15310495914</v>
+      </c>
+      <c r="BC48">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="49" spans="1:29">
+    <row r="49" spans="1:55">
       <c r="W49" t="s">
         <v>195</v>
       </c>
@@ -4771,8 +5634,20 @@
       <c r="AC49">
         <v>339561526035</v>
       </c>
+      <c r="AW49" t="s">
+        <v>230</v>
+      </c>
+      <c r="AZ49">
+        <v>2007</v>
+      </c>
+      <c r="BA49">
+        <v>16206118071</v>
+      </c>
+      <c r="BC49">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="50" spans="1:29">
+    <row r="50" spans="1:55">
       <c r="A50">
         <v>9</v>
       </c>
@@ -4841,8 +5716,20 @@
       <c r="AC50">
         <v>339561526035</v>
       </c>
+      <c r="AW50" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ50">
+        <v>2008</v>
+      </c>
+      <c r="BA50">
+        <v>19482936409</v>
+      </c>
+      <c r="BC50">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="51" spans="1:29">
+    <row r="51" spans="1:55">
       <c r="A51">
         <v>9</v>
       </c>
@@ -4912,8 +5799,27 @@
       <c r="AC51">
         <v>339561526035</v>
       </c>
+      <c r="AW51" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AX51">
+        <v>385498</v>
+      </c>
+      <c r="AY51">
+        <f t="shared" ref="AY51:AY52" si="4">AX51/BC51</f>
+        <v>1.1352817396640665E-6</v>
+      </c>
+      <c r="AZ51" t="s">
+        <v>205</v>
+      </c>
+      <c r="BA51">
+        <v>339561526035</v>
+      </c>
+      <c r="BC51">
+        <v>339561526035</v>
+      </c>
     </row>
-    <row r="52" spans="1:29">
+    <row r="52" spans="1:55">
       <c r="A52">
         <v>9</v>
       </c>
@@ -4963,8 +5869,17 @@
       <c r="T52" t="s">
         <v>175</v>
       </c>
+      <c r="AW52" t="s">
+        <v>197</v>
+      </c>
+      <c r="AX52">
+        <v>15734124</v>
+      </c>
+      <c r="AY52">
+        <v>4.6336592321646651E-5</v>
+      </c>
     </row>
-    <row r="53" spans="1:29">
+    <row r="53" spans="1:55">
       <c r="A53">
         <v>9</v>
       </c>
@@ -5015,7 +5930,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:29">
+    <row r="54" spans="1:55">
       <c r="A54">
         <v>9</v>
       </c>
@@ -5045,24 +5960,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:29">
+    <row r="56" spans="1:55">
       <c r="B56" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:29">
+    <row r="57" spans="1:55">
       <c r="B57" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:29">
+    <row r="58" spans="1:55">
       <c r="B58" s="4" t="s">
         <v>190</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="V1:V58">
-    <sortCondition ref="V1:V58"/>
+  <sortState ref="AW1:AW58">
+    <sortCondition ref="AW1:AW58"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
added a bunch of graphs for the basiclevels frequency analysis and 2bin length analysis
</commit_message>
<xml_diff>
--- a/Caroline/Stimuli_Experiment2_version2/stimuliOverview.xlsx
+++ b/Caroline/Stimuli_Experiment2_version2/stimuliOverview.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-1060" yWindow="20" windowWidth="13680" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="11580" yWindow="180" windowWidth="13680" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="293">
   <si>
     <t>target</t>
   </si>
@@ -835,13 +835,76 @@
   </si>
   <si>
     <t>catfish</t>
+  </si>
+  <si>
+    <t>bedsideTable</t>
+  </si>
+  <si>
+    <t>blackBear</t>
+  </si>
+  <si>
+    <t>clownFish</t>
+  </si>
+  <si>
+    <t>coffeeTable</t>
+  </si>
+  <si>
+    <t>diningTable</t>
+  </si>
+  <si>
+    <t>GermanShepherd</t>
+  </si>
+  <si>
+    <t>goldFish</t>
+  </si>
+  <si>
+    <t>grizzlyBear</t>
+  </si>
+  <si>
+    <t>hawaiiShirt</t>
+  </si>
+  <si>
+    <t>mnMs</t>
+  </si>
+  <si>
+    <t>pandaBear</t>
+  </si>
+  <si>
+    <t>picnicTable</t>
+  </si>
+  <si>
+    <t>polarBear</t>
+  </si>
+  <si>
+    <t>poloShirt</t>
+  </si>
+  <si>
+    <t>skittles</t>
+  </si>
+  <si>
+    <t>suv</t>
+  </si>
+  <si>
+    <t>swordFish</t>
+  </si>
+  <si>
+    <t>tShirt</t>
+  </si>
+  <si>
+    <t>2gram</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>also 1gram</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -891,6 +954,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -909,7 +977,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="173">
+  <cellStyleXfs count="177">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1083,8 +1151,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1093,8 +1165,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="173">
+  <cellStyles count="177">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1181,6 +1254,8 @@
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1267,6 +1342,8 @@
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1596,10 +1673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC58"/>
+  <dimension ref="A1:BD58"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="AS18" workbookViewId="0">
-      <selection activeCell="AY26" sqref="AY26"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BD1" sqref="BD1:BD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1607,11 +1684,11 @@
     <col min="24" max="24" width="13.6640625" customWidth="1"/>
     <col min="25" max="25" width="17.5" customWidth="1"/>
     <col min="27" max="27" width="28.6640625" customWidth="1"/>
-    <col min="51" max="51" width="14.33203125" customWidth="1"/>
-    <col min="53" max="53" width="16.83203125" customWidth="1"/>
+    <col min="52" max="52" width="14.33203125" customWidth="1"/>
+    <col min="54" max="54" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55">
+    <row r="1" spans="1:56">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -1696,20 +1773,26 @@
       <c r="AT1" t="s">
         <v>269</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AV1" t="s">
+        <v>290</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>292</v>
+      </c>
+      <c r="AY1" t="s">
         <v>204</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>206</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>270</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:55">
+    <row r="2" spans="1:56">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1796,26 +1879,26 @@
       <c r="AQ2" t="s">
         <v>259</v>
       </c>
-      <c r="AW2" t="s">
+      <c r="AX2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="AX2">
+      <c r="AY2">
         <v>39951249</v>
       </c>
-      <c r="AY2">
+      <c r="AZ2">
         <v>1.1765540538854234E-4</v>
       </c>
-      <c r="AZ2">
+      <c r="BA2">
         <v>1960</v>
       </c>
-      <c r="BA2">
+      <c r="BB2">
         <v>2341981521</v>
       </c>
-      <c r="BC2">
+      <c r="BD2">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="3" spans="1:55">
+    <row r="3" spans="1:56">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1899,20 +1982,20 @@
       <c r="AQ3" t="s">
         <v>260</v>
       </c>
-      <c r="AW3" t="s">
+      <c r="AX3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="AZ3">
+      <c r="BA3">
         <v>1961</v>
       </c>
-      <c r="BA3">
+      <c r="BB3">
         <v>2567977722</v>
       </c>
-      <c r="BC3">
+      <c r="BD3">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:56">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1996,20 +2079,23 @@
       <c r="AQ4" t="s">
         <v>261</v>
       </c>
-      <c r="AW4" t="s">
-        <v>243</v>
-      </c>
-      <c r="AZ4">
+      <c r="AV4" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>272</v>
+      </c>
+      <c r="BA4">
         <v>1962</v>
       </c>
-      <c r="BA4">
+      <c r="BB4">
         <v>2818694749</v>
       </c>
-      <c r="BC4">
+      <c r="BD4">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:56">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2093,20 +2179,20 @@
       <c r="AQ5" t="s">
         <v>262</v>
       </c>
-      <c r="AW5" t="s">
+      <c r="AX5" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="AZ5">
+      <c r="BA5">
         <v>1963</v>
       </c>
-      <c r="BA5">
+      <c r="BB5">
         <v>2955051696</v>
       </c>
-      <c r="BC5">
+      <c r="BD5">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="6" spans="1:55">
+    <row r="6" spans="1:56">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2172,20 +2258,23 @@
       <c r="AM6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="AW6" t="s">
-        <v>218</v>
-      </c>
-      <c r="AZ6">
+      <c r="AV6" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX6" t="s">
+        <v>273</v>
+      </c>
+      <c r="BA6">
         <v>1964</v>
       </c>
-      <c r="BA6">
+      <c r="BB6">
         <v>2931038992</v>
       </c>
-      <c r="BC6">
+      <c r="BD6">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="7" spans="1:55">
+    <row r="7" spans="1:56">
       <c r="W7" t="s">
         <v>147</v>
       </c>
@@ -2217,20 +2306,20 @@
       <c r="AM7" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="AW7" t="s">
+      <c r="AX7" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="AZ7">
+      <c r="BA7">
         <v>1965</v>
       </c>
-      <c r="BA7">
+      <c r="BB7">
         <v>3300623502</v>
       </c>
-      <c r="BC7">
+      <c r="BD7">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="8" spans="1:55">
+    <row r="8" spans="1:56">
       <c r="A8">
         <v>2</v>
       </c>
@@ -2311,20 +2400,20 @@
       <c r="AM8" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="AW8" t="s">
+      <c r="AX8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AZ8">
+      <c r="BA8">
         <v>1966</v>
       </c>
-      <c r="BA8">
+      <c r="BB8">
         <v>3466842517</v>
       </c>
-      <c r="BC8">
+      <c r="BD8">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="9" spans="1:55">
+    <row r="9" spans="1:56">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2405,20 +2494,20 @@
       <c r="AM9" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="AW9" t="s">
+      <c r="AX9" t="s">
         <v>271</v>
       </c>
-      <c r="AZ9">
+      <c r="BA9">
         <v>1967</v>
       </c>
-      <c r="BA9">
+      <c r="BB9">
         <v>3658119990</v>
       </c>
-      <c r="BC9">
+      <c r="BD9">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="10" spans="1:55">
+    <row r="10" spans="1:56">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2502,26 +2591,26 @@
       <c r="AM10" t="s">
         <v>252</v>
       </c>
-      <c r="AW10" t="s">
+      <c r="AX10" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="AX10">
+      <c r="AY10">
         <v>7987510</v>
       </c>
-      <c r="AY10">
+      <c r="AZ10">
         <v>2.3523012436858629E-5</v>
       </c>
-      <c r="AZ10">
+      <c r="BA10">
         <v>1968</v>
       </c>
-      <c r="BA10">
+      <c r="BB10">
         <v>3968752101</v>
       </c>
-      <c r="BC10">
+      <c r="BD10">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="11" spans="1:55">
+    <row r="11" spans="1:56">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2602,20 +2691,26 @@
       <c r="AM11" t="s">
         <v>253</v>
       </c>
+      <c r="AV11" t="s">
+        <v>291</v>
+      </c>
       <c r="AW11" t="s">
-        <v>237</v>
-      </c>
-      <c r="AZ11">
+        <v>291</v>
+      </c>
+      <c r="AX11" t="s">
+        <v>274</v>
+      </c>
+      <c r="BA11">
         <v>1969</v>
       </c>
-      <c r="BA11">
+      <c r="BB11">
         <v>3942222509</v>
       </c>
-      <c r="BC11">
+      <c r="BD11">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="12" spans="1:55">
+    <row r="12" spans="1:56">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2675,20 +2770,23 @@
       <c r="AM12" t="s">
         <v>254</v>
       </c>
-      <c r="AW12" t="s">
-        <v>241</v>
-      </c>
-      <c r="AZ12">
+      <c r="AV12" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX12" t="s">
+        <v>275</v>
+      </c>
+      <c r="BA12">
         <v>1970</v>
       </c>
-      <c r="BA12">
+      <c r="BB12">
         <v>4086393350</v>
       </c>
-      <c r="BC12">
+      <c r="BD12">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="13" spans="1:55">
+    <row r="13" spans="1:56">
       <c r="W13" t="s">
         <v>48</v>
       </c>
@@ -2720,20 +2818,20 @@
       <c r="AM13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AW13" t="s">
+      <c r="AX13" t="s">
         <v>221</v>
       </c>
-      <c r="AZ13">
+      <c r="BA13">
         <v>1971</v>
       </c>
-      <c r="BA13">
+      <c r="BB13">
         <v>4058576649</v>
       </c>
-      <c r="BC13">
+      <c r="BD13">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="14" spans="1:55">
+    <row r="14" spans="1:56">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2817,27 +2915,27 @@
       <c r="AM14" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="AW14" s="3" t="s">
+      <c r="AX14" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AX14">
+      <c r="AY14">
         <v>1142904</v>
       </c>
-      <c r="AY14">
-        <f>AX14/BC13</f>
+      <c r="AZ14">
+        <f>AY14/BD13</f>
         <v>3.3658230169521507E-6</v>
       </c>
-      <c r="AZ14">
+      <c r="BA14">
         <v>1972</v>
       </c>
-      <c r="BA14">
+      <c r="BB14">
         <v>4174172415</v>
       </c>
-      <c r="BC14">
+      <c r="BD14">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="15" spans="1:55">
+    <row r="15" spans="1:56">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2918,26 +3016,26 @@
       <c r="AM15" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="AW15" s="3" t="s">
+      <c r="AX15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AX15">
+      <c r="AY15">
         <v>49602</v>
       </c>
-      <c r="AY15">
+      <c r="AZ15">
         <v>1.4607661998458365E-7</v>
       </c>
-      <c r="AZ15">
+      <c r="BA15">
         <v>1973</v>
       </c>
-      <c r="BA15">
+      <c r="BB15">
         <v>4058707895</v>
       </c>
-      <c r="BC15">
+      <c r="BD15">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="16" spans="1:55">
+    <row r="16" spans="1:56">
       <c r="A16">
         <v>3</v>
       </c>
@@ -3018,20 +3116,23 @@
       <c r="AM16" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="AW16" t="s">
-        <v>242</v>
-      </c>
-      <c r="AZ16">
+      <c r="AV16" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX16" t="s">
+        <v>276</v>
+      </c>
+      <c r="BA16">
         <v>1974</v>
       </c>
-      <c r="BA16">
+      <c r="BB16">
         <v>4045487401</v>
       </c>
-      <c r="BC16">
+      <c r="BD16">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="17" spans="1:55">
+    <row r="17" spans="1:56">
       <c r="A17">
         <v>3</v>
       </c>
@@ -3112,27 +3213,27 @@
       <c r="AM17" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="AW17" t="s">
+      <c r="AX17" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="AX17">
+      <c r="AY17">
         <v>21789518</v>
       </c>
-      <c r="AY17">
-        <f>AX17/BC16</f>
+      <c r="AZ17">
+        <f>AY17/BD16</f>
         <v>6.4169572608629595E-5</v>
       </c>
-      <c r="AZ17">
+      <c r="BA17">
         <v>1975</v>
       </c>
-      <c r="BA17">
+      <c r="BB17">
         <v>4104379941</v>
       </c>
-      <c r="BC17">
+      <c r="BD17">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="18" spans="1:55">
+    <row r="18" spans="1:56">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3195,20 +3296,20 @@
       <c r="AM18" t="s">
         <v>98</v>
       </c>
-      <c r="AW18" t="s">
+      <c r="AX18" t="s">
         <v>144</v>
       </c>
-      <c r="AZ18">
+      <c r="BA18">
         <v>1976</v>
       </c>
-      <c r="BA18">
+      <c r="BB18">
         <v>4242326406</v>
       </c>
-      <c r="BC18">
+      <c r="BD18">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="19" spans="1:55">
+    <row r="19" spans="1:56">
       <c r="W19" t="s">
         <v>7</v>
       </c>
@@ -3240,20 +3341,20 @@
       <c r="AM19" t="s">
         <v>99</v>
       </c>
-      <c r="AW19" t="s">
+      <c r="AX19" t="s">
         <v>231</v>
       </c>
-      <c r="AZ19">
+      <c r="BA19">
         <v>1977</v>
       </c>
-      <c r="BA19">
+      <c r="BB19">
         <v>4314577619</v>
       </c>
-      <c r="BC19">
+      <c r="BD19">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="20" spans="1:55">
+    <row r="20" spans="1:56">
       <c r="A20">
         <v>4</v>
       </c>
@@ -3334,20 +3435,20 @@
       <c r="AM20" t="s">
         <v>100</v>
       </c>
-      <c r="AW20" t="s">
+      <c r="AX20" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="AZ20">
+      <c r="BA20">
         <v>1978</v>
       </c>
-      <c r="BA20">
+      <c r="BB20">
         <v>4365839878</v>
       </c>
-      <c r="BC20">
+      <c r="BD20">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="21" spans="1:55">
+    <row r="21" spans="1:56">
       <c r="A21">
         <v>4</v>
       </c>
@@ -3428,27 +3529,27 @@
       <c r="AM21" t="s">
         <v>267</v>
       </c>
-      <c r="AW21" t="s">
+      <c r="AX21" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="AX21">
+      <c r="AY21">
         <v>16497919</v>
       </c>
-      <c r="AY21">
-        <f>AX21/BC20</f>
+      <c r="AZ21">
+        <f>AY21/BD20</f>
         <v>4.8585949040350033E-5</v>
       </c>
-      <c r="AZ21">
+      <c r="BA21">
         <v>1979</v>
       </c>
-      <c r="BA21">
+      <c r="BB21">
         <v>4528331460</v>
       </c>
-      <c r="BC21">
+      <c r="BD21">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="22" spans="1:55">
+    <row r="22" spans="1:56">
       <c r="A22">
         <v>4</v>
       </c>
@@ -3532,26 +3633,26 @@
       <c r="AM22" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AW22" t="s">
+      <c r="AX22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="AX22">
+      <c r="AY22">
         <v>6098822</v>
       </c>
-      <c r="AY22">
+      <c r="AZ22">
         <v>1.7960874635047345E-5</v>
       </c>
-      <c r="AZ22">
+      <c r="BA22">
         <v>1980</v>
       </c>
-      <c r="BA22">
+      <c r="BB22">
         <v>4611609946</v>
       </c>
-      <c r="BC22">
+      <c r="BD22">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="23" spans="1:55">
+    <row r="23" spans="1:56">
       <c r="A23">
         <v>4</v>
       </c>
@@ -3633,27 +3734,27 @@
       <c r="AM23" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="AW23" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="AX23">
+      <c r="AX23" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="AY23" s="6">
         <v>97790</v>
       </c>
-      <c r="AY23">
-        <f>AX23/BC22</f>
+      <c r="AZ23" s="6">
+        <f>AY23/BD22</f>
         <v>2.8798904617338887E-7</v>
       </c>
-      <c r="AZ23">
+      <c r="BA23">
         <v>1981</v>
       </c>
-      <c r="BA23">
+      <c r="BB23">
         <v>4627406112</v>
       </c>
-      <c r="BC23">
+      <c r="BD23">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="24" spans="1:55">
+    <row r="24" spans="1:56">
       <c r="A24">
         <v>4</v>
       </c>
@@ -3714,20 +3815,26 @@
       <c r="AM24" s="3" t="s">
         <v>133</v>
       </c>
+      <c r="AV24" t="s">
+        <v>291</v>
+      </c>
       <c r="AW24" t="s">
-        <v>239</v>
-      </c>
-      <c r="AZ24">
+        <v>291</v>
+      </c>
+      <c r="AX24" t="s">
+        <v>278</v>
+      </c>
+      <c r="BA24">
         <v>1982</v>
       </c>
-      <c r="BA24">
+      <c r="BB24">
         <v>4839530894</v>
       </c>
-      <c r="BC24">
+      <c r="BD24">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="25" spans="1:55">
+    <row r="25" spans="1:56">
       <c r="W25" t="s">
         <v>194</v>
       </c>
@@ -3760,20 +3867,23 @@
       <c r="AM25" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="AW25" t="s">
-        <v>216</v>
-      </c>
-      <c r="AZ25">
+      <c r="AV25" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX25" t="s">
+        <v>279</v>
+      </c>
+      <c r="BA25">
         <v>1983</v>
       </c>
-      <c r="BA25">
+      <c r="BB25">
         <v>4982167985</v>
       </c>
-      <c r="BC25">
+      <c r="BD25">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="26" spans="1:55">
+    <row r="26" spans="1:56">
       <c r="A26">
         <v>5</v>
       </c>
@@ -3857,20 +3967,26 @@
       <c r="AM26" t="s">
         <v>246</v>
       </c>
+      <c r="AV26" t="s">
+        <v>291</v>
+      </c>
       <c r="AW26" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX26" t="s">
         <v>223</v>
       </c>
-      <c r="AZ26">
+      <c r="BA26">
         <v>1984</v>
       </c>
-      <c r="BA26">
+      <c r="BB26">
         <v>5309222580</v>
       </c>
-      <c r="BC26">
+      <c r="BD26">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="27" spans="1:55">
+    <row r="27" spans="1:56">
       <c r="A27">
         <v>5</v>
       </c>
@@ -3951,20 +4067,23 @@
       <c r="AM27" t="s">
         <v>268</v>
       </c>
-      <c r="AW27" t="s">
-        <v>235</v>
-      </c>
-      <c r="AZ27">
+      <c r="AV27" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX27" t="s">
+        <v>280</v>
+      </c>
+      <c r="BA27">
         <v>1985</v>
       </c>
-      <c r="BA27">
+      <c r="BB27">
         <v>5475269397</v>
       </c>
-      <c r="BC27">
+      <c r="BD27">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="28" spans="1:55">
+    <row r="28" spans="1:56">
       <c r="A28">
         <v>5</v>
       </c>
@@ -4045,20 +4164,26 @@
       <c r="AM28" t="s">
         <v>247</v>
       </c>
+      <c r="AV28" t="s">
+        <v>291</v>
+      </c>
       <c r="AW28" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX28" t="s">
         <v>232</v>
       </c>
-      <c r="AZ28">
+      <c r="BA28">
         <v>1986</v>
       </c>
-      <c r="BA28">
+      <c r="BB28">
         <v>5793946882</v>
       </c>
-      <c r="BC28">
+      <c r="BD28">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="29" spans="1:55">
+    <row r="29" spans="1:56">
       <c r="A29">
         <v>5</v>
       </c>
@@ -4139,27 +4264,27 @@
       <c r="AM29" t="s">
         <v>248</v>
       </c>
-      <c r="AW29" s="3" t="s">
+      <c r="AX29" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="AX29">
+      <c r="AY29">
         <v>76741</v>
       </c>
-      <c r="AY29">
-        <f>AX29/BC28</f>
+      <c r="AZ29">
+        <f>AY29/BD28</f>
         <v>2.2600028011444968E-7</v>
       </c>
-      <c r="AZ29">
+      <c r="BA29">
         <v>1987</v>
       </c>
-      <c r="BA29">
+      <c r="BB29">
         <v>5936558026</v>
       </c>
-      <c r="BC29">
+      <c r="BD29">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="30" spans="1:55">
+    <row r="30" spans="1:56">
       <c r="A30">
         <v>5</v>
       </c>
@@ -4222,20 +4347,26 @@
       <c r="AM30" t="s">
         <v>249</v>
       </c>
+      <c r="AV30" t="s">
+        <v>291</v>
+      </c>
       <c r="AW30" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX30" t="s">
         <v>225</v>
       </c>
-      <c r="AZ30">
+      <c r="BA30">
         <v>1988</v>
       </c>
-      <c r="BA30">
+      <c r="BB30">
         <v>6191886939</v>
       </c>
-      <c r="BC30">
+      <c r="BD30">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="31" spans="1:55">
+    <row r="31" spans="1:56">
       <c r="W31" t="s">
         <v>67</v>
       </c>
@@ -4267,20 +4398,20 @@
       <c r="AM31" t="s">
         <v>250</v>
       </c>
-      <c r="AW31" t="s">
-        <v>226</v>
-      </c>
-      <c r="AZ31">
+      <c r="AX31" t="s">
+        <v>281</v>
+      </c>
+      <c r="BA31">
         <v>1989</v>
       </c>
-      <c r="BA31">
+      <c r="BB31">
         <v>6549339038</v>
       </c>
-      <c r="BC31">
+      <c r="BD31">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="32" spans="1:55">
+    <row r="32" spans="1:56">
       <c r="A32">
         <v>6</v>
       </c>
@@ -4361,20 +4492,20 @@
       <c r="AM32" t="s">
         <v>251</v>
       </c>
-      <c r="AW32" t="s">
+      <c r="AX32" t="s">
         <v>256</v>
       </c>
-      <c r="AZ32">
+      <c r="BA32">
         <v>1990</v>
       </c>
-      <c r="BA32">
+      <c r="BB32">
         <v>7075013106</v>
       </c>
-      <c r="BC32">
+      <c r="BD32">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="33" spans="1:55">
+    <row r="33" spans="1:56">
       <c r="A33">
         <v>6</v>
       </c>
@@ -4458,20 +4589,23 @@
       <c r="AM33" t="s">
         <v>266</v>
       </c>
-      <c r="AW33" t="s">
-        <v>220</v>
-      </c>
-      <c r="AZ33">
+      <c r="AV33" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX33" t="s">
+        <v>282</v>
+      </c>
+      <c r="BA33">
         <v>1991</v>
       </c>
-      <c r="BA33">
+      <c r="BB33">
         <v>6895715366</v>
       </c>
-      <c r="BC33">
+      <c r="BD33">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="34" spans="1:55">
+    <row r="34" spans="1:56">
       <c r="A34">
         <v>6</v>
       </c>
@@ -4560,20 +4694,20 @@
       <c r="AM34" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="AW34" t="s">
+      <c r="AX34" t="s">
         <v>233</v>
       </c>
-      <c r="AZ34">
+      <c r="BA34">
         <v>1992</v>
       </c>
-      <c r="BA34">
+      <c r="BB34">
         <v>7596808027</v>
       </c>
-      <c r="BC34">
+      <c r="BD34">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="35" spans="1:55">
+    <row r="35" spans="1:56">
       <c r="A35">
         <v>6</v>
       </c>
@@ -4654,20 +4788,23 @@
       <c r="AM35" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="AW35" t="s">
-        <v>240</v>
-      </c>
-      <c r="AZ35">
+      <c r="AV35" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX35" t="s">
+        <v>283</v>
+      </c>
+      <c r="BA35">
         <v>1993</v>
       </c>
-      <c r="BA35">
+      <c r="BB35">
         <v>7492130348</v>
       </c>
-      <c r="BC35">
+      <c r="BD35">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="36" spans="1:55">
+    <row r="36" spans="1:56">
       <c r="A36">
         <v>6</v>
       </c>
@@ -4730,20 +4867,20 @@
       <c r="AM36" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="AW36" t="s">
+      <c r="AX36" t="s">
         <v>234</v>
       </c>
-      <c r="AZ36">
+      <c r="BA36">
         <v>1994</v>
       </c>
-      <c r="BA36">
+      <c r="BB36">
         <v>8027353540</v>
       </c>
-      <c r="BC36">
+      <c r="BD36">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="37" spans="1:55">
+    <row r="37" spans="1:56">
       <c r="B37" t="s">
         <v>182</v>
       </c>
@@ -4781,26 +4918,26 @@
       <c r="AM37" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="AW37" t="s">
+      <c r="AX37" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="AX37">
+      <c r="AY37">
         <v>52852109</v>
       </c>
-      <c r="AY37">
+      <c r="AZ37">
         <v>1.5564810777341222E-4</v>
       </c>
-      <c r="AZ37">
+      <c r="BA37">
         <v>1995</v>
       </c>
-      <c r="BA37">
+      <c r="BB37">
         <v>8276258599</v>
       </c>
-      <c r="BC37">
+      <c r="BD37">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="38" spans="1:55">
+    <row r="38" spans="1:56">
       <c r="A38">
         <v>7</v>
       </c>
@@ -4866,20 +5003,23 @@
       <c r="AC38">
         <v>339561526035</v>
       </c>
-      <c r="AW38" t="s">
-        <v>217</v>
-      </c>
-      <c r="AZ38">
+      <c r="AV38" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX38" t="s">
+        <v>284</v>
+      </c>
+      <c r="BA38">
         <v>1996</v>
       </c>
-      <c r="BA38">
+      <c r="BB38">
         <v>8745049453</v>
       </c>
-      <c r="BC38">
+      <c r="BD38">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="39" spans="1:55">
+    <row r="39" spans="1:56">
       <c r="A39">
         <v>7</v>
       </c>
@@ -4945,20 +5085,23 @@
       <c r="AC39">
         <v>339561526035</v>
       </c>
-      <c r="AW39" t="s">
-        <v>229</v>
-      </c>
-      <c r="AZ39">
+      <c r="AV39" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX39" t="s">
+        <v>285</v>
+      </c>
+      <c r="BA39">
         <v>1997</v>
       </c>
-      <c r="BA39">
+      <c r="BB39">
         <v>8979708108</v>
       </c>
-      <c r="BC39">
+      <c r="BD39">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="40" spans="1:55">
+    <row r="40" spans="1:56">
       <c r="A40">
         <v>7</v>
       </c>
@@ -5021,27 +5164,27 @@
       <c r="AC40">
         <v>339561526035</v>
       </c>
-      <c r="AW40" s="3" t="s">
+      <c r="AX40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AX40">
+      <c r="AY40">
         <v>121280</v>
       </c>
-      <c r="AY40">
-        <f t="shared" ref="AY40" si="1">AX40/BC40</f>
+      <c r="AZ40">
+        <f t="shared" ref="AZ40" si="1">AY40/BD40</f>
         <v>3.5716649473267821E-7</v>
       </c>
-      <c r="AZ40">
+      <c r="BA40">
         <v>1998</v>
       </c>
-      <c r="BA40">
+      <c r="BB40">
         <v>9406708249</v>
       </c>
-      <c r="BC40">
+      <c r="BD40">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="41" spans="1:55">
+    <row r="41" spans="1:56">
       <c r="A41">
         <v>7</v>
       </c>
@@ -5104,27 +5247,27 @@
       <c r="AC41">
         <v>339561526035</v>
       </c>
-      <c r="AW41" s="3" t="s">
+      <c r="AX41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="AX41">
+      <c r="AY41">
         <v>8595412</v>
       </c>
-      <c r="AY41">
-        <f t="shared" ref="AY41" si="2">AX41/BC41</f>
+      <c r="AZ41">
+        <f t="shared" ref="AZ41" si="2">AY41/BD41</f>
         <v>2.5313268262064634E-5</v>
       </c>
-      <c r="AZ41">
+      <c r="BA41">
         <v>1999</v>
       </c>
-      <c r="BA41">
+      <c r="BB41">
         <v>9997156197</v>
       </c>
-      <c r="BC41">
+      <c r="BD41">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="42" spans="1:55">
+    <row r="42" spans="1:56">
       <c r="A42">
         <v>7</v>
       </c>
@@ -5172,20 +5315,20 @@
       <c r="AC42">
         <v>339561526035</v>
       </c>
-      <c r="AW42" t="s">
+      <c r="AX42" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="AZ42">
+      <c r="BA42">
         <v>2000</v>
       </c>
-      <c r="BA42">
+      <c r="BB42">
         <v>11190986329</v>
       </c>
-      <c r="BC42">
+      <c r="BD42">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="43" spans="1:55">
+    <row r="43" spans="1:56">
       <c r="W43" t="s">
         <v>37</v>
       </c>
@@ -5205,20 +5348,20 @@
       <c r="AC43">
         <v>339561526035</v>
       </c>
-      <c r="AW43" t="s">
-        <v>224</v>
-      </c>
-      <c r="AZ43">
+      <c r="AX43" t="s">
+        <v>286</v>
+      </c>
+      <c r="BA43">
         <v>2001</v>
       </c>
-      <c r="BA43">
+      <c r="BB43">
         <v>11349375656</v>
       </c>
-      <c r="BC43">
+      <c r="BD43">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="44" spans="1:55">
+    <row r="44" spans="1:56">
       <c r="A44">
         <v>8</v>
       </c>
@@ -5287,20 +5430,20 @@
       <c r="AC44">
         <v>339561526035</v>
       </c>
-      <c r="AW44" t="s">
+      <c r="AX44" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="AZ44">
+      <c r="BA44">
         <v>2002</v>
       </c>
-      <c r="BA44">
+      <c r="BB44">
         <v>12519922882</v>
       </c>
-      <c r="BC44">
+      <c r="BD44">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="45" spans="1:55">
+    <row r="45" spans="1:56">
       <c r="A45">
         <v>8</v>
       </c>
@@ -5369,20 +5512,23 @@
       <c r="AC45">
         <v>339561526035</v>
       </c>
-      <c r="AW45" t="s">
+      <c r="AV45" t="s">
+        <v>291</v>
+      </c>
+      <c r="AX45" t="s">
         <v>257</v>
       </c>
-      <c r="AZ45">
+      <c r="BA45">
         <v>2003</v>
       </c>
-      <c r="BA45">
+      <c r="BB45">
         <v>13632028136</v>
       </c>
-      <c r="BC45">
+      <c r="BD45">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="46" spans="1:55">
+    <row r="46" spans="1:56">
       <c r="A46">
         <v>8</v>
       </c>
@@ -5451,27 +5597,27 @@
       <c r="AC46">
         <v>339561526035</v>
       </c>
-      <c r="AW46" s="3" t="s">
+      <c r="AX46" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AX46">
+      <c r="AY46">
         <v>583171</v>
       </c>
-      <c r="AY46">
-        <f t="shared" ref="AY46" si="3">AX46/BC46</f>
+      <c r="AZ46">
+        <f t="shared" ref="AZ46" si="3">AY46/BD46</f>
         <v>1.7174236634214271E-6</v>
       </c>
-      <c r="AZ46">
+      <c r="BA46">
         <v>2004</v>
       </c>
-      <c r="BA46">
+      <c r="BB46">
         <v>14705541576</v>
       </c>
-      <c r="BC46">
+      <c r="BD46">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="47" spans="1:55">
+    <row r="47" spans="1:56">
       <c r="A47">
         <v>8</v>
       </c>
@@ -5540,20 +5686,20 @@
       <c r="AC47">
         <v>339561526035</v>
       </c>
-      <c r="AW47" t="s">
-        <v>222</v>
-      </c>
-      <c r="AZ47">
+      <c r="AX47" t="s">
+        <v>287</v>
+      </c>
+      <c r="BA47">
         <v>2005</v>
       </c>
-      <c r="BA47">
+      <c r="BB47">
         <v>14425183957</v>
       </c>
-      <c r="BC47">
+      <c r="BD47">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="48" spans="1:55">
+    <row r="48" spans="1:56">
       <c r="A48">
         <v>8</v>
       </c>
@@ -5601,20 +5747,26 @@
       <c r="AC48">
         <v>339561526035</v>
       </c>
+      <c r="AV48" t="s">
+        <v>291</v>
+      </c>
       <c r="AW48" t="s">
-        <v>238</v>
-      </c>
-      <c r="AZ48">
+        <v>291</v>
+      </c>
+      <c r="AX48" t="s">
+        <v>288</v>
+      </c>
+      <c r="BA48">
         <v>2006</v>
       </c>
-      <c r="BA48">
+      <c r="BB48">
         <v>15310495914</v>
       </c>
-      <c r="BC48">
+      <c r="BD48">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="49" spans="1:55">
+    <row r="49" spans="1:56">
       <c r="W49" t="s">
         <v>195</v>
       </c>
@@ -5634,20 +5786,20 @@
       <c r="AC49">
         <v>339561526035</v>
       </c>
-      <c r="AW49" t="s">
-        <v>230</v>
-      </c>
-      <c r="AZ49">
+      <c r="AX49" t="s">
+        <v>289</v>
+      </c>
+      <c r="BA49">
         <v>2007</v>
       </c>
-      <c r="BA49">
+      <c r="BB49">
         <v>16206118071</v>
       </c>
-      <c r="BC49">
+      <c r="BD49">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="50" spans="1:55">
+    <row r="50" spans="1:56">
       <c r="A50">
         <v>9</v>
       </c>
@@ -5716,20 +5868,20 @@
       <c r="AC50">
         <v>339561526035</v>
       </c>
-      <c r="AW50" t="s">
+      <c r="AX50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AZ50">
+      <c r="BA50">
         <v>2008</v>
       </c>
-      <c r="BA50">
+      <c r="BB50">
         <v>19482936409</v>
       </c>
-      <c r="BC50">
+      <c r="BD50">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="51" spans="1:55">
+    <row r="51" spans="1:56">
       <c r="A51">
         <v>9</v>
       </c>
@@ -5799,27 +5951,27 @@
       <c r="AC51">
         <v>339561526035</v>
       </c>
-      <c r="AW51" s="3" t="s">
+      <c r="AX51" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AX51">
+      <c r="AY51">
         <v>385498</v>
       </c>
-      <c r="AY51">
-        <f t="shared" ref="AY51:AY52" si="4">AX51/BC51</f>
+      <c r="AZ51">
+        <f t="shared" ref="AZ51" si="4">AY51/BD51</f>
         <v>1.1352817396640665E-6</v>
       </c>
-      <c r="AZ51" t="s">
+      <c r="BA51" t="s">
         <v>205</v>
       </c>
-      <c r="BA51">
-        <v>339561526035</v>
-      </c>
-      <c r="BC51">
+      <c r="BB51">
+        <v>339561526035</v>
+      </c>
+      <c r="BD51">
         <v>339561526035</v>
       </c>
     </row>
-    <row r="52" spans="1:55">
+    <row r="52" spans="1:56">
       <c r="A52">
         <v>9</v>
       </c>
@@ -5869,17 +6021,17 @@
       <c r="T52" t="s">
         <v>175</v>
       </c>
-      <c r="AW52" t="s">
+      <c r="AX52" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="AX52">
+      <c r="AY52">
         <v>15734124</v>
       </c>
-      <c r="AY52">
+      <c r="AZ52">
         <v>4.6336592321646651E-5</v>
       </c>
     </row>
-    <row r="53" spans="1:55">
+    <row r="53" spans="1:56">
       <c r="A53">
         <v>9</v>
       </c>
@@ -5930,7 +6082,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="54" spans="1:55">
+    <row r="54" spans="1:56">
       <c r="A54">
         <v>9</v>
       </c>
@@ -5960,24 +6112,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:55">
+    <row r="56" spans="1:56">
       <c r="B56" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="57" spans="1:55">
+    <row r="57" spans="1:56">
       <c r="B57" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="58" spans="1:55">
+    <row r="58" spans="1:56">
       <c r="B58" s="4" t="s">
         <v>190</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="AW1:AW58">
-    <sortCondition ref="AW1:AW58"/>
+  <sortState ref="AX1:AX58">
+    <sortCondition ref="AX1:AX58"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>